<commit_message>
fix salad text in vi, fix menu in mobile view and drink image size
</commit_message>
<xml_diff>
--- a/public/data/menu.xlsx
+++ b/public/data/menu.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="330">
   <si>
     <t>Category</t>
   </si>
@@ -117,7 +117,7 @@
     <t>nấm bào ngư, tàu hủ ki, rau thơm các loại, xốt gỏi chua cay</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/khaivi%2FGo%CC%89i%20na%CC%82%CC%81m%20ba%CC%80o%20ngu%CC%9B%20xe%CC%81%20tro%CC%A3%CC%82n_%20khaivi.jpg?alt=media&amp;token=ad85f3fa-c32c-4d96-8404-9275edd7cbb3</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/khaivi%2FGo%CC%89i%20na%CC%82%CC%81m%20ba%CC%80o%20ngu%CC%9B%20xe%CC%81%20tro%CC%A3%CC%82n_%20khaivi.jpg?alt=media&amp;token=afb1b5fc-4db0-4562-88cd-75c1ddc67200</t>
   </si>
   <si>
     <t>GỎI somtum thái lan</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">Lotus Delight Salad </t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/khaivi%2FGo%CC%89i%20ngo%CC%81%20sen_khaivi.jpg?alt=media&amp;token=20ceda2b-3410-4a1e-be24-41204e4bd339</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/khaivi%2FGo%CC%89i%20ngo%CC%81%20sen_khaivi.jpg?alt=media&amp;token=5e637b3c-4647-440e-9a9b-7c7a3a9c72b3</t>
   </si>
   <si>
     <t>GỎI RONG SỤN</t>
@@ -201,7 +201,7 @@
     <t>Summer Roll</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FGo%CC%89i%20cuo%CC%82%CC%81n_moncuon.jpg?alt=media&amp;token=cfd5053e-4dd9-460b-b0be-e5e4588f89f3</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FGo%CC%89i%20cuo%CC%82%CC%81n_moncuon.jpg?alt=media&amp;token=07605767-b35d-4d6e-99b0-62f8fb4edd53</t>
   </si>
   <si>
     <t>bì cuốn</t>
@@ -213,7 +213,7 @@
     <t>Crystal Autumn Roll</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FBi%CC%80%20cuo%CC%82%CC%81n_moncuon.jpg?alt=media&amp;token=90e99629-1a1e-4868-9854-3af4e4cf4b0a</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FBi%CC%80%20cuo%CC%82%CC%81n_moncuon.jpg?alt=media&amp;token=eb987c96-df54-461d-a485-5125061ea01f</t>
   </si>
   <si>
     <t>mẹt cuốn</t>
@@ -225,6 +225,9 @@
     <t>Veggie Wrap &amp; Roll</t>
   </si>
   <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FMe%CC%A3t%20cuo%CC%82%CC%81n_moncuon.jpg?alt=media&amp;token=5f2bbf4c-bc70-4803-b68e-776a513ffdd6</t>
+  </si>
+  <si>
     <t>bánh xèo</t>
   </si>
   <si>
@@ -234,7 +237,7 @@
     <t>Vietnamese Pancake</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FBa%CC%81nh%20xe%CC%80o_moncuon.jpg?alt=media&amp;token=da8f0b06-3cd9-4b20-9fed-5542759ac1c2</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/moncuon%2FBa%CC%81nh%20xe%CC%80o_moncuon.jpg?alt=media&amp;token=7425fff4-9c1c-4105-95c2-379f5bce4f53</t>
   </si>
   <si>
     <t>Nấm nướng lá lốt</t>
@@ -339,7 +342,7 @@
     <t>Thai fried rice with pineapple</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monchinh%2FCo%CC%9Bm%20chie%CC%82n%20tho%CC%9Bm%20kie%CC%82%CC%89u%20Tha%CC%81i_monchinh.jpg?alt=media&amp;token=6215990f-7a2b-4cdf-a2a3-60c87c6f0f1a</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monchinh%2FCo%CC%9Bm%20chie%CC%82n%20tho%CC%9Bm%20kie%CC%82%CC%89u%20Tha%CC%81i_monchinh.jpg?alt=media&amp;token=045f1bc7-ed11-48c2-8675-54a91eb22fae</t>
   </si>
   <si>
     <t>cơm chiên dương châu</t>
@@ -351,6 +354,9 @@
     <t>Yang Chow fried rice</t>
   </si>
   <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monchinh%2FCo%CC%9Bm%20chie%CC%82n%20du%CC%9Bo%CC%9Bng%20cha%CC%82u_monchinh.jpg?alt=media&amp;token=e4003164-d386-4f50-b8ab-47f3b9f24699</t>
+  </si>
+  <si>
     <t>cơm trộn hàn quốc</t>
   </si>
   <si>
@@ -360,7 +366,7 @@
     <t>korean mixed rice</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monchinh%2FCo%CC%9Bm%20tro%CC%A3%CC%82n%20Ha%CC%80n%20Quo%CC%82%CC%81c_monchinh.jpg?alt=media&amp;token=a4271614-8131-4539-9616-ecadd73a9091</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monchinh%2FCo%CC%9Bm%20tro%CC%A3%CC%82n%20Ha%CC%80n%20Quo%CC%82%CC%81c_monchinh.jpg?alt=media&amp;token=37e45fe4-94e0-48e9-a3c8-28a441007484</t>
   </si>
   <si>
     <t>cơm nấm lúc lắc &amp; canh rau củ</t>
@@ -576,7 +582,7 @@
     <t>Mapo Tofu</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20non%20so%CC%82%CC%81t%20tu%CC%9B%CC%81%20xuye%CC%82n_monman.jpg?alt=media&amp;token=cb5318e9-1e5d-44dd-b18f-5cf9e92634dc</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20non%20so%CC%82%CC%81t%20tu%CC%9B%CC%81%20xuye%CC%82n_monman.jpg?alt=media&amp;token=127fdafd-749c-4f24-82bf-c0a0f086f3f7</t>
   </si>
   <si>
     <t>ĐẬU HỦ CHƯNG TƯƠNG</t>
@@ -585,7 +591,7 @@
     <t>Steamed Tofu with Salted Soybean Sauce</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20chu%CC%9Bng%20tu%CC%9Bo%CC%9Bng_monman.jpg?alt=media&amp;token=0702e508-980a-4a53-9deb-0c0a3330b705</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20chu%CC%9Bng%20tu%CC%9Bo%CC%9Bng_monman.jpg?alt=media&amp;token=75a7c087-59c9-4ee6-a01e-8f6f4f85a9da</t>
   </si>
   <si>
     <t>ĐẬU HỦ XỐC SA TẾ</t>
@@ -594,7 +600,7 @@
     <t>Satay Tofu</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20xo%CC%82%CC%81c%20sa%20te%CC%82%CC%81_monman.jpg?alt=media&amp;token=969ae59d-1ca5-4f11-b928-ec655b170c36</t>
+    <t>https://firebasestorage.googleapis.com/v0/b/dieuthien-production.appspot.com/o/monman%2F%C4%90a%CC%A3%CC%82u%20hu%CC%83%20xo%CC%82%CC%81c%20sa%20te%CC%82%CC%81_monman.jpg?alt=media&amp;token=65951195-23c9-48f6-b738-618a4cbaf70a</t>
   </si>
   <si>
     <t>NẤM RƠM KHO TIÊU</t>
@@ -1559,8 +1565,8 @@
         <v>noodles, bean sprouts, chives, fried tofu, fried mushrooms, tamarind sauce, served with roasted peanuts, chili, and lemon.</v>
       </c>
       <c r="G2" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B2,""vi"",""zh"")"),"泰式炒河粉")</f>
-        <v>泰式炒河粉</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B2,""vi"",""zh"")"),"泰语PAD")</f>
+        <v>泰语PAD</v>
       </c>
       <c r="H2" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D2&lt;&gt;"""", GOOGLETRANSLATE(D2, ""vi"", ""zh""), """")
@@ -1790,7 +1796,7 @@
         <v>34</v>
       </c>
       <c r="C8" s="6">
-        <v>55001.0</v>
+        <v>59000.0</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>35</v>
@@ -1831,7 +1837,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="6">
-        <v>55002.0</v>
+        <v>55000.0</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>39</v>
@@ -1872,7 +1878,7 @@
         <v>42</v>
       </c>
       <c r="C10" s="6">
-        <v>55003.0</v>
+        <v>55000.0</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>43</v>
@@ -2005,8 +2011,8 @@
       </c>
       <c r="F13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D13&lt;&gt;"""", GOOGLETRANSLATE(D13, ""vi"", ""en""), """")
-"),"Stuffed with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce")</f>
-        <v>Stuffed with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce</v>
+"),"Filled with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce")</f>
+        <v>Filled with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce</v>
       </c>
       <c r="G13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""vi"",""zh"")"),"春卷")</f>
@@ -2014,8 +2020,8 @@
       </c>
       <c r="H13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D13&lt;&gt;"""", GOOGLETRANSLATE(D13, ""vi"", ""zh""), """")
-"),"塞满什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露")</f>
-        <v>塞满什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露</v>
+"),"馅料为什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露")</f>
+        <v>馅料为什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>57</v>
@@ -2055,8 +2061,8 @@
       </c>
       <c r="H14" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D14&lt;&gt;"""", GOOGLETRANSLATE(D14, ""vi"", ""zh""), """")
-"),"新鲜粉丝馅，什锦香草，拌炒蘑菇，配花生酱")</f>
-        <v>新鲜粉丝馅，什锦香草，拌炒蘑菇，配花生酱</v>
+"),"新鲜粉丝馅，什锦香草，炒蘑菇配花生酱")</f>
+        <v>新鲜粉丝馅，什锦香草，炒蘑菇配花生酱</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>61</v>
@@ -2091,8 +2097,8 @@
         <v>Filled with assorted potatoes, taro, vermicelli, assorted herbs, served with sweet and sour fish sauce</v>
       </c>
       <c r="G15" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""vi"",""zh"")"),"包装卷")</f>
-        <v>包装卷</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B15,""vi"",""zh"")"),"卷信封")</f>
+        <v>卷信封</v>
       </c>
       <c r="H15" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D15&lt;&gt;"""", GOOGLETRANSLATE(D15, ""vi"", ""zh""), """")
@@ -2141,7 +2147,7 @@
         <v>鲜粉米纸卷、什锦生菜、蚝油蘑菇、花生酱</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="J16" s="9" t="b">
         <v>0</v>
@@ -2156,16 +2162,16 @@
         <v>53</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="6">
         <v>55000.0</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F17" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D17&lt;&gt;"""", GOOGLETRANSLATE(D17, ""vi"", ""en""), """")
@@ -2173,8 +2179,8 @@
         <v>stuffed with bean sprouts, carrots, mixed stir-fried mushrooms, green beans, rolled with assorted raw vegetables, served with sweet and sour fish sauce.</v>
       </c>
       <c r="G17" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B17,""vi"",""zh"")"),"薄煎饼")</f>
-        <v>薄煎饼</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B17,""vi"",""zh"")"),"班赫西奥")</f>
+        <v>班赫西奥</v>
       </c>
       <c r="H17" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D17&lt;&gt;"""", GOOGLETRANSLATE(D17, ""vi"", ""zh""), """")
@@ -2182,7 +2188,7 @@
         <v>里面塞满了豆芽、胡萝卜、炒蘑菇、青豆，卷上什锦生蔬菜，配上糖醋鱼露。</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J17" s="9" t="b">
         <v>0</v>
@@ -2197,16 +2203,16 @@
         <v>53</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6">
         <v>55000.0</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F18" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D18&lt;&gt;"""", GOOGLETRANSLATE(D18, ""vi"", ""en""), """")
@@ -2223,7 +2229,7 @@
         <v>罗勒叶卷炒什锦蘑菇，卷上米纸，配上新鲜粉丝，什锦生菜，配上素食调味酱</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J18" s="9" t="b">
         <v>0</v>
@@ -2235,24 +2241,24 @@
     </row>
     <row r="19" ht="36.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C19" s="6">
         <v>150000.0</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F19" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D19&lt;&gt;"""", GOOGLETRANSLATE(D19, ""vi"", ""en""), """")
-"),"green pepper hotpot ; vegetable spinach ; vegetables cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; enokitake ; Young tofu ; Served with vegetarian fish sauce and fresh vermicelli")</f>
-        <v>green pepper hotpot ; vegetable spinach ; vegetables cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; enokitake ; Young tofu ; Served with vegetarian fish sauce and fresh vermicelli</v>
+"),"green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushrooms ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli")</f>
+        <v>green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushrooms ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli</v>
       </c>
       <c r="G19" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""vi"",""zh"")"),"青椒蘑菇火锅")</f>
@@ -2260,11 +2266,11 @@
       </c>
       <c r="H19" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D19&lt;&gt;"""", GOOGLETRANSLATE(D19, ""vi"", ""zh""), """")
-"),"青椒火锅；蔬菜菠菜；蔬菜 卷心菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；金针菇；嫩豆腐；配素食鱼露和新鲜粉丝")</f>
-        <v>青椒火锅；蔬菜菠菜；蔬菜 卷心菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；金针菇；嫩豆腐；配素食鱼露和新鲜粉丝</v>
+"),"青椒火锅；菠菜 ;大白菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；金针菇；软豆腐；配素食鱼露和新鲜粉丝")</f>
+        <v>青椒火锅；菠菜 ;大白菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；金针菇；软豆腐；配素食鱼露和新鲜粉丝</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J19" s="9" t="b">
         <v>0</v>
@@ -2276,24 +2282,24 @@
     </row>
     <row r="20" ht="36.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C20" s="6">
         <v>150000.0</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F20" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D20&lt;&gt;"""", GOOGLETRANSLATE(D20, ""vi"", ""en""), """")
-"),"Thai hotpot ; banana vegetables ; vegetables cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; enokitake ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli")</f>
-        <v>Thai hotpot ; banana vegetables ; vegetables cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; enokitake ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli</v>
+"),"Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushrooms ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli")</f>
+        <v>Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushrooms ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli</v>
       </c>
       <c r="G20" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""vi"",""zh"")"),"泰式火锅")</f>
@@ -2301,11 +2307,11 @@
       </c>
       <c r="H20" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D20&lt;&gt;"""", GOOGLETRANSLATE(D20, ""vi"", ""zh""), """")
-"),"泰式火锅；香蕉蔬菜；蔬菜 卷心菜；菠菜 ;蔬菜需要水；鸡腿蘑菇；金针菇；鲍鱼蘑菇；软豆腐配素鱼露和新鲜粉丝")</f>
-        <v>泰式火锅；香蕉蔬菜；蔬菜 卷心菜；菠菜 ;蔬菜需要水；鸡腿蘑菇；金针菇；鲍鱼蘑菇；软豆腐配素鱼露和新鲜粉丝</v>
+"),"泰式火锅；香蕉蔬菜；大白菜；菠菜 ;蔬菜需要水；鸡腿蘑菇；金针菇；鲍鱼蘑菇；软豆腐配素鱼露和新鲜粉丝")</f>
+        <v>泰式火锅；香蕉蔬菜；大白菜；菠菜 ;蔬菜需要水；鸡腿蘑菇；金针菇；鲍鱼蘑菇；软豆腐配素鱼露和新鲜粉丝</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J20" s="9" t="b">
         <v>0</v>
@@ -2317,24 +2323,24 @@
     </row>
     <row r="21" ht="36.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" s="6">
         <v>150000.0</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F21" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D21&lt;&gt;"""", GOOGLETRANSLATE(D21, ""vi"", ""en""), """")
-"),"satay hotpot ; vegetable spinach ; vegetables cabbage ; abalone mushrooms ; chicken drumstick mushrooms ; black enoki mushroom ; Tofu ; Tofu ki served with satay fish sauce and fresh vermicelli")</f>
-        <v>satay hotpot ; vegetable spinach ; vegetables cabbage ; abalone mushrooms ; chicken drumstick mushrooms ; black enoki mushroom ; Tofu ; Tofu ki served with satay fish sauce and fresh vermicelli</v>
+"),"satay hotpot ; spinach ; Chinese cabbage ; abalone mushrooms ; chicken drumstick mushrooms ; black enoki mushroom ; tofu ; Tofu ki served with satay fish sauce and fresh vermicelli")</f>
+        <v>satay hotpot ; spinach ; Chinese cabbage ; abalone mushrooms ; chicken drumstick mushrooms ; black enoki mushroom ; tofu ; Tofu ki served with satay fish sauce and fresh vermicelli</v>
       </c>
       <c r="G21" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B21,""vi"",""zh"")"),"很棒的沙爹火锅")</f>
@@ -2342,11 +2348,11 @@
       </c>
       <c r="H21" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D21&lt;&gt;"""", GOOGLETRANSLATE(D21, ""vi"", ""zh""), """")
-"),"沙爹火锅；蔬菜菠菜；蔬菜 卷心菜；鲍鱼蘑菇；鸡腿蘑菇；黑金针菇；豆腐 ;豆腐记配沙爹鱼露和新鲜粉丝")</f>
-        <v>沙爹火锅；蔬菜菠菜；蔬菜 卷心菜；鲍鱼蘑菇；鸡腿蘑菇；黑金针菇；豆腐 ;豆腐记配沙爹鱼露和新鲜粉丝</v>
+"),"沙爹火锅；菠菜 ;大白菜；鲍鱼蘑菇；鸡腿蘑菇；黑金针菇；豆腐；豆腐记配沙爹鱼露和新鲜粉丝")</f>
+        <v>沙爹火锅；菠菜 ;大白菜；鲍鱼蘑菇；鸡腿蘑菇；黑金针菇；豆腐；豆腐记配沙爹鱼露和新鲜粉丝</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J21" s="13" t="b">
         <v>0</v>
@@ -2358,24 +2364,24 @@
     </row>
     <row r="22" ht="36.75" customHeight="1">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C22" s="6">
         <v>150000.0</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F22" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D22&lt;&gt;"""", GOOGLETRANSLATE(D22, ""vi"", ""en""), """")
-"),"chao hotpot ; vegetable spinach ; vegetables cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Tofu ki served with vegetarian dipping sauce and fresh vermicelli")</f>
-        <v>chao hotpot ; vegetable spinach ; vegetables cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Tofu ki served with vegetarian dipping sauce and fresh vermicelli</v>
+"),"chao hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Tofu ki served with vegetarian dipping sauce and fresh vermicelli")</f>
+        <v>chao hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Tofu ki served with vegetarian dipping sauce and fresh vermicelli</v>
       </c>
       <c r="G22" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B22,""vi"",""zh"")"),"潮火锅")</f>
@@ -2383,11 +2389,11 @@
       </c>
       <c r="H22" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D22&lt;&gt;"""", GOOGLETRANSLATE(D22, ""vi"", ""zh""), """")
-"),"潮火锅;蔬菜菠菜；蔬菜 卷心菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；豆腐木配素食蘸酱和新鲜粉丝")</f>
-        <v>潮火锅;蔬菜菠菜；蔬菜 卷心菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；豆腐木配素食蘸酱和新鲜粉丝</v>
+"),"潮火锅;菠菜 ;大白菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；豆腐木配素食蘸酱和新鲜粉丝")</f>
+        <v>潮火锅;菠菜 ;大白菜；芥菜；鸡腿蘑菇；鲍鱼蘑菇；豆腐木配素食蘸酱和新鲜粉丝</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J22" s="9" t="b">
         <v>0</v>
@@ -2399,16 +2405,16 @@
     </row>
     <row r="23" ht="36.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C23" s="6">
         <v>150000.0</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>13</v>
@@ -2428,7 +2434,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J23" s="9" t="b">
         <v>0</v>
@@ -2440,17 +2446,17 @@
     </row>
     <row r="24" ht="36.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="6">
         <v>250000.0</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D24&lt;&gt;"""", GOOGLETRANSLATE(D24, ""vi"", ""en""), """")
@@ -2467,7 +2473,7 @@
         <v/>
       </c>
       <c r="I24" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J24" s="9" t="b">
         <v>0</v>
@@ -2479,19 +2485,19 @@
     </row>
     <row r="25" ht="36.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C25" s="6">
         <v>55000.0</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F25" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D25&lt;&gt;"""", GOOGLETRANSLATE(D25, ""vi"", ""en""), """")
@@ -2504,11 +2510,11 @@
       </c>
       <c r="H25" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D25&lt;&gt;"""", GOOGLETRANSLATE(D25, ""vi"", ""zh""), """")
-"),"白饭、素咸鱼、素肉松、素紫菜、葱（适量）")</f>
-        <v>白饭、素咸鱼、素肉松、素紫菜、葱（适量）</v>
+"),"米饭、素咸鱼、素肉松、素紫菜、葱（适量）")</f>
+        <v>米饭、素咸鱼、素肉松、素紫菜、葱（适量）</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J25" s="9" t="b">
         <v>0</v>
@@ -2520,19 +2526,19 @@
     </row>
     <row r="26" ht="36.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C26" s="6">
         <v>55000.0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F26" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D26&lt;&gt;"""", GOOGLETRANSLATE(D26, ""vi"", ""en""), """")
@@ -2549,7 +2555,7 @@
         <v>大米、菠萝、青豆、胡萝卜、美国玉米、大葱（可调）</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J26" s="9" t="b">
         <v>0</v>
@@ -2561,19 +2567,19 @@
     </row>
     <row r="27" ht="36.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C27" s="6">
         <v>55000.0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F27" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D27&lt;&gt;"""", GOOGLETRANSLATE(D27, ""vi"", ""en""), """")
@@ -2590,7 +2596,7 @@
         <v>阳州炒饭：米饭、青豆、胡萝卜、美国玉米、大葱（可调节）</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="J27" s="9" t="b">
         <v>0</v>
@@ -2602,19 +2608,19 @@
     </row>
     <row r="28" ht="36.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C28" s="6">
         <v>59000.0</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F28" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D28&lt;&gt;"""", GOOGLETRANSLATE(D28, ""vi"", ""en""), """")
@@ -2631,7 +2637,7 @@
         <v>米饭、豆芽、紫甘蓝、彩椒、美国玉米、芝麻花生、炒蘑菇，配韩式拌饭酱</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J28" s="9" t="b">
         <v>0</v>
@@ -2643,19 +2649,19 @@
     </row>
     <row r="29" ht="36.75" customHeight="1">
       <c r="A29" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C29" s="6">
         <v>55000.0</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F29" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D29&lt;&gt;"""", GOOGLETRANSLATE(D29, ""vi"", ""en""), """")
@@ -2672,7 +2678,7 @@
         <v>米饭、鸡腿菇、青椒、洋葱、炒蒜、奶昔配蔬菜汤</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J29" s="9" t="b">
         <v>0</v>
@@ -2684,19 +2690,19 @@
     </row>
     <row r="30" ht="36.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C30" s="6">
         <v>55000.0</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F30" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D30&lt;&gt;"""", GOOGLETRANSLATE(D30, ""vi"", ""en""), """")
@@ -2713,7 +2719,7 @@
         <v>米饭、鸡腿菇、红薯、胡萝卜、芋头、椰奶、咖喱香料，配蔬菜汤</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J30" s="9" t="b">
         <v>0</v>
@@ -2725,16 +2731,16 @@
     </row>
     <row r="31" ht="36.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C31" s="6">
         <v>55000.0</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>13</v>
@@ -2745,8 +2751,8 @@
         <v>Korean vermicelli, bok choy, purple cabbage, carrots, fried abalone mushrooms, mixed vermicelli sauce.</v>
       </c>
       <c r="G31" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B31,""vi"",""zh"")"),"拌面")</f>
-        <v>拌面</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B31,""vi"",""zh"")"),"混合诗句")</f>
+        <v>混合诗句</v>
       </c>
       <c r="H31" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D31&lt;&gt;"""", GOOGLETRANSLATE(D31, ""vi"", ""zh""), """")
@@ -2754,7 +2760,7 @@
         <v>韩国粉丝，白菜，紫甘蓝，胡萝卜，炒鲍鱼菇，混合粉丝酱。</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J31" s="9" t="b">
         <v>1</v>
@@ -2766,16 +2772,16 @@
     </row>
     <row r="32" ht="36.75" customHeight="1">
       <c r="A32" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C32" s="6">
         <v>55000.0</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E32" s="7" t="s">
         <v>13</v>
@@ -2795,7 +2801,7 @@
         <v>米粉，青椒，大白菜，洋葱，大白菜，炒豆腐，炒蘑菇，炒蒜。</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J32" s="9" t="b">
         <v>0</v>
@@ -2807,16 +2813,16 @@
     </row>
     <row r="33" ht="36.75" customHeight="1">
       <c r="A33" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C33" s="6">
         <v>55000.0</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E33" s="7" t="s">
         <v>13</v>
@@ -2836,7 +2842,7 @@
         <v>黄面，青椒，大白菜，洋葱，大白菜，炒豆腐，炒蘑菇，炒洋葱。</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J33" s="9" t="b">
         <v>0</v>
@@ -2848,16 +2854,16 @@
     </row>
     <row r="34" ht="36.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C34" s="6">
         <v>59000.0</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>13</v>
@@ -2877,7 +2883,7 @@
         <v>意大利面、鸡腿蘑菇、番茄酱、</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J34" s="9" t="b">
         <v>0</v>
@@ -2889,10 +2895,10 @@
     </row>
     <row r="35" ht="36.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C35" s="6">
         <v>65000.0</v>
@@ -2916,7 +2922,7 @@
         <v/>
       </c>
       <c r="I35" s="8" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J35" s="9" t="b">
         <v>0</v>
@@ -2928,10 +2934,10 @@
     </row>
     <row r="36" ht="36.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C36" s="6">
         <v>65000.0</v>
@@ -2955,7 +2961,7 @@
         <v/>
       </c>
       <c r="I36" s="8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="J36" s="9" t="b">
         <v>0</v>
@@ -2967,17 +2973,17 @@
     </row>
     <row r="37" ht="36.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C37" s="6">
         <v>150000.0</v>
       </c>
       <c r="D37" s="11"/>
       <c r="E37" s="7" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F37" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D37&lt;&gt;"""", GOOGLETRANSLATE(D37, ""vi"", ""en""), """")
@@ -2994,7 +3000,7 @@
         <v/>
       </c>
       <c r="I37" s="8" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="J37" s="9" t="b">
         <v>0</v>
@@ -3006,19 +3012,19 @@
     </row>
     <row r="38" ht="36.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C38" s="6">
         <v>150000.0</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F38" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D38&lt;&gt;"""", GOOGLETRANSLATE(D38, ""vi"", ""en""), """")
@@ -3035,7 +3041,7 @@
         <v>鲍鱼菇、港盐 配蛋黄酱和辣椒酱</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="J38" s="9" t="b">
         <v>1</v>
@@ -3047,19 +3053,19 @@
     </row>
     <row r="39" ht="36.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C39" s="6">
         <v>50000.0</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="F39" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D39&lt;&gt;"""", GOOGLETRANSLATE(D39, ""vi"", ""en""), """")
@@ -3076,7 +3082,7 @@
         <v>海藻;豆腐、鲍鱼菇、胡萝卜、炸洋葱；胡椒、生姜</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J39" s="9" t="b">
         <v>0</v>
@@ -3088,19 +3094,19 @@
     </row>
     <row r="40" ht="36.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C40" s="6">
         <v>50000.0</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F40" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D40&lt;&gt;"""", GOOGLETRANSLATE(D40, ""vi"", ""en""), """")
@@ -3117,7 +3123,7 @@
         <v>薄荷、秋葵、豆芽、西红柿、菠萝、香草、炒大蒜</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="J40" s="9" t="b">
         <v>0</v>
@@ -3129,19 +3135,19 @@
     </row>
     <row r="41" ht="36.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C41" s="6">
         <v>50000.0</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F41" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D41&lt;&gt;"""", GOOGLETRANSLATE(D41, ""vi"", ""en""), """")
@@ -3158,7 +3164,7 @@
         <v>青芥菜、鲍鱼菇、生姜、胡椒</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="J41" s="9" t="b">
         <v>0</v>
@@ -3170,36 +3176,36 @@
     </row>
     <row r="42" ht="36.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C42" s="6">
         <v>39000.0</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="F42" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D42&lt;&gt;"""", GOOGLETRANSLATE(D42, ""vi"", ""en""), """")
-"),"fairy's hair ; American corn ; carrot ; mushroom ; string bean ; fried onion ; pepper ; coriander")</f>
-        <v>fairy's hair ; American corn ; carrot ; mushroom ; string bean ; fried onion ; pepper ; coriander</v>
+"),"fairy hair ; American corn ; carrot ; mushroom ; string beans ; onions ; pepper ; coriander")</f>
+        <v>fairy hair ; American corn ; carrot ; mushroom ; string beans ; onions ; pepper ; coriander</v>
       </c>
       <c r="G42" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""vi"",""zh"")"),"TOC天汤")</f>
-        <v>TOC天汤</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""vi"",""zh"")"),"东天汤")</f>
+        <v>东天汤</v>
       </c>
       <c r="H42" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D42&lt;&gt;"""", GOOGLETRANSLATE(D42, ""vi"", ""zh""), """")
-"),"仙女的头发；美国玉米；胡萝卜 ;蘑菇 ;四季豆；炒洋葱；胡椒 ;香菜")</f>
-        <v>仙女的头发；美国玉米；胡萝卜 ;蘑菇 ;四季豆；炒洋葱；胡椒 ;香菜</v>
+"),"仙女的头发；美国玉米；胡萝卜 ;蘑菇;四季豆；洋葱；胡椒;香菜")</f>
+        <v>仙女的头发；美国玉米；胡萝卜 ;蘑菇;四季豆；洋葱；胡椒;香菜</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J42" s="9" t="b">
         <v>0</v>
@@ -3211,24 +3217,24 @@
     </row>
     <row r="43" ht="36.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C43" s="6">
         <v>39000.0</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="F43" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D43&lt;&gt;"""", GOOGLETRANSLATE(D43, ""vi"", ""en""), """")
-"),"White wood-ear mushroom ; Lotus seeds ; carrot mushrooms ; string bean ; fried onion ; pepper; Coriander.")</f>
-        <v>White wood-ear mushroom ; Lotus seeds ; carrot mushrooms ; string bean ; fried onion ; pepper; Coriander.</v>
+"),"snow mushroom ; lotus seeds ; carrot mushrooms ; string beans ; onions ; pepper; Coriander.")</f>
+        <v>snow mushroom ; lotus seeds ; carrot mushrooms ; string beans ; onions ; pepper; Coriander.</v>
       </c>
       <c r="G43" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B43,""vi"",""zh"")"),"雪菇莲子汤")</f>
@@ -3236,11 +3242,11 @@
       </c>
       <c r="H43" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D43&lt;&gt;"""", GOOGLETRANSLATE(D43, ""vi"", ""zh""), """")
-"),"白木耳；莲子；胡萝卜蘑菇；四季豆；炒洋葱；胡椒;香菜。")</f>
-        <v>白木耳；莲子；胡萝卜蘑菇；四季豆；炒洋葱；胡椒;香菜。</v>
+"),"雪蘑菇；莲子；胡萝卜蘑菇；四季豆；洋葱；胡椒;香菜。")</f>
+        <v>雪蘑菇；莲子；胡萝卜蘑菇；四季豆；洋葱；胡椒;香菜。</v>
       </c>
       <c r="I43" s="14" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J43" s="9" t="b">
         <v>0</v>
@@ -3252,19 +3258,19 @@
     </row>
     <row r="44" ht="36.75" customHeight="1">
       <c r="A44" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C44" s="6">
         <v>45000.0</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F44" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D44&lt;&gt;"""", GOOGLETRANSLATE(D44, ""vi"", ""en""), """")
@@ -3272,8 +3278,8 @@
         <v>kimchi hotpot ; purple cabbage ; Chinese cabbage ; Abalone mushrooms served with Korean noodles</v>
       </c>
       <c r="G44" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""vi"",""zh"")"),"蒜炒菠菜")</f>
-        <v>蒜炒菠菜</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B44,""vi"",""zh"")"),"蒜炒米纳赫")</f>
+        <v>蒜炒米纳赫</v>
       </c>
       <c r="H44" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D44&lt;&gt;"""", GOOGLETRANSLATE(D44, ""vi"", ""zh""), """")
@@ -3281,7 +3287,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I44" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="J44" s="9" t="b">
         <v>0</v>
@@ -3293,19 +3299,19 @@
     </row>
     <row r="45" ht="36.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C45" s="6">
         <v>55000.0</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F45" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D45&lt;&gt;"""", GOOGLETRANSLATE(D45, ""vi"", ""en""), """")
@@ -3322,7 +3328,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I45" s="14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="J45" s="9" t="b">
         <v>0</v>
@@ -3334,19 +3340,19 @@
     </row>
     <row r="46" ht="36.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C46" s="6">
         <v>55000.0</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F46" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D46&lt;&gt;"""", GOOGLETRANSLATE(D46, ""vi"", ""en""), """")
@@ -3354,8 +3360,8 @@
         <v>kimchi hotpot ; purple cabbage ; Chinese cabbage ; Abalone mushrooms served with Korean noodles</v>
       </c>
       <c r="G46" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""vi"",""zh"")"),"什锦炒蔬菜")</f>
-        <v>什锦炒蔬菜</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B46,""vi"",""zh"")"),"什锦蔬菜")</f>
+        <v>什锦蔬菜</v>
       </c>
       <c r="H46" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D46&lt;&gt;"""", GOOGLETRANSLATE(D46, ""vi"", ""zh""), """")
@@ -3363,7 +3369,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I46" s="14" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="J46" s="9" t="b">
         <v>0</v>
@@ -3375,19 +3381,19 @@
     </row>
     <row r="47" ht="36.75" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C47" s="6">
         <v>55000.0</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F47" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D47&lt;&gt;"""", GOOGLETRANSLATE(D47, ""vi"", ""en""), """")
@@ -3404,7 +3410,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I47" s="14" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J47" s="9" t="b">
         <v>0</v>
@@ -3416,19 +3422,19 @@
     </row>
     <row r="48" ht="36.75" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C48" s="6">
         <v>55000.0</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="F48" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D48&lt;&gt;"""", GOOGLETRANSLATE(D48, ""vi"", ""en""), """")
@@ -3445,7 +3451,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I48" s="14" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="J48" s="9" t="b">
         <v>0</v>
@@ -3457,19 +3463,19 @@
     </row>
     <row r="49" ht="36.75" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C49" s="6">
         <v>65000.0</v>
       </c>
       <c r="D49" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F49" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D49&lt;&gt;"""", GOOGLETRANSLATE(D49, ""vi"", ""en""), """")
@@ -3486,7 +3492,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I49" s="14" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="J49" s="9" t="b">
         <v>0</v>
@@ -3498,19 +3504,19 @@
     </row>
     <row r="50" ht="36.75" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C50" s="6">
         <v>55000.0</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="F50" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D50&lt;&gt;"""", GOOGLETRANSLATE(D50, ""vi"", ""en""), """")
@@ -3527,7 +3533,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I50" s="14" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J50" s="9" t="b">
         <v>0</v>
@@ -3539,19 +3545,19 @@
     </row>
     <row r="51" ht="36.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C51" s="6">
         <v>55000.0</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F51" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D51&lt;&gt;"""", GOOGLETRANSLATE(D51, ""vi"", ""en""), """")
@@ -3568,7 +3574,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I51" s="14" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="J51" s="9" t="b">
         <v>0</v>
@@ -3580,19 +3586,19 @@
     </row>
     <row r="52" ht="36.75" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C52" s="6">
         <v>55000.0</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F52" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D52&lt;&gt;"""", GOOGLETRANSLATE(D52, ""vi"", ""en""), """")
@@ -3609,7 +3615,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="J52" s="9" t="b">
         <v>0</v>
@@ -3621,19 +3627,19 @@
     </row>
     <row r="53" ht="36.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C53" s="6">
         <v>65000.0</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F53" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D53&lt;&gt;"""", GOOGLETRANSLATE(D53, ""vi"", ""en""), """")
@@ -3650,7 +3656,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I53" s="14" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J53" s="9" t="b">
         <v>0</v>
@@ -3662,19 +3668,19 @@
     </row>
     <row r="54" ht="36.75" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C54" s="6">
         <v>65000.0</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="F54" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D54&lt;&gt;"""", GOOGLETRANSLATE(D54, ""vi"", ""en""), """")
@@ -3691,7 +3697,7 @@
         <v>泡菜火锅；紫甘蓝;大白菜；鲍鱼蘑菇配韩式面条</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J54" s="9" t="b">
         <v>0</v>
@@ -3703,24 +3709,24 @@
     </row>
     <row r="55" ht="36.75" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C55" s="6">
         <v>35000.0</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F55" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D55&lt;&gt;"""", GOOGLETRANSLATE(D55, ""vi"", ""en""), """")
-"),"Weak snow; snow lotus ; peach resin ; Goji berries ; Red Apple ; Longan")</f>
-        <v>Weak snow; snow lotus ; peach resin ; Goji berries ; Red Apple ; Longan</v>
+"),"Weak snow; snow lotus ; peach resin ; Goji berries ; red apple ; Longan")</f>
+        <v>Weak snow; snow lotus ; peach resin ; Goji berries ; red apple ; Longan</v>
       </c>
       <c r="G55" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B55,""vi"",""zh"")"),"燕窝雪茶美容养颜")</f>
@@ -3728,11 +3734,11 @@
       </c>
       <c r="H55" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D55&lt;&gt;"""", GOOGLETRANSLATE(D55, ""vi"", ""zh""), """")
-"),"雪弱；雪莲花；桃胶；枸杞子；红苹果 ;龙眼")</f>
-        <v>雪弱；雪莲花；桃胶；枸杞子；红苹果 ;龙眼</v>
+"),"雪弱；雪莲花；桃胶；枸杞子；红苹果;龙眼")</f>
+        <v>雪弱；雪莲花；桃胶；枸杞子；红苹果;龙眼</v>
       </c>
       <c r="I55" s="14" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J55" s="9" t="b">
         <v>0</v>
@@ -3744,24 +3750,24 @@
     </row>
     <row r="56" ht="36.75" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C56" s="6">
         <v>35000.0</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F56" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D56&lt;&gt;"""", GOOGLETRANSLATE(D56, ""vi"", ""en""), """")
-"),"Lotus seeds; Goji berries ; Red Apple ; Cordyceps")</f>
-        <v>Lotus seeds; Goji berries ; Red Apple ; Cordyceps</v>
+"),"lotus seeds; Goji berries ; red apple ; Cordyceps")</f>
+        <v>lotus seeds; Goji berries ; red apple ; Cordyceps</v>
       </c>
       <c r="G56" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B56,""vi"",""zh"")"),"虫草莲子茶")</f>
@@ -3769,11 +3775,11 @@
       </c>
       <c r="H56" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D56&lt;&gt;"""", GOOGLETRANSLATE(D56, ""vi"", ""zh""), """")
-"),"莲子；枸杞子；红苹果 ;虫草")</f>
-        <v>莲子；枸杞子；红苹果 ;虫草</v>
+"),"莲子；枸杞子；红苹果;虫草")</f>
+        <v>莲子；枸杞子；红苹果;虫草</v>
       </c>
       <c r="I56" s="14" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="J56" s="9" t="b">
         <v>0</v>
@@ -3785,24 +3791,24 @@
     </row>
     <row r="57" ht="36.75" customHeight="1">
       <c r="A57" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C57" s="6">
         <v>35000.0</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="F57" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D57&lt;&gt;"""", GOOGLETRANSLATE(D57, ""vi"", ""en""), """")
-"),"yogurt ; mulberry level ; rim occlusion level; grinded ice")</f>
-        <v>yogurt ; mulberry level ; rim occlusion level; grinded ice</v>
+"),"yogurt ; mulberry level ; rim occlusion level; shaved ice")</f>
+        <v>yogurt ; mulberry level ; rim occlusion level; shaved ice</v>
       </c>
       <c r="G57" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B57,""vi"",""zh"")"),"桑葚酸奶")</f>
@@ -3810,11 +3816,11 @@
       </c>
       <c r="H57" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D57&lt;&gt;"""", GOOGLETRANSLATE(D57, ""vi"", ""zh""), """")
-"),"酸奶 ;桑葚级；边缘咬合程度；碎冰")</f>
-        <v>酸奶 ;桑葚级；边缘咬合程度；碎冰</v>
+"),"酸奶 ;桑葚级；边缘咬合程度；刨冰")</f>
+        <v>酸奶 ;桑葚级；边缘咬合程度；刨冰</v>
       </c>
       <c r="I57" s="14" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="J57" s="9" t="b">
         <v>0</v>
@@ -3826,16 +3832,16 @@
     </row>
     <row r="58" ht="36.75" customHeight="1">
       <c r="A58" s="4" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C58" s="6">
         <v>12000.0</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="E58" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B58,""vi"",""en"")"),"Panna Cotta (Blueberry, passion fruit, guava, peach, mulberry)")</f>
@@ -3856,7 +3862,7 @@
         <v>由纯豆浆制成；明胶配水果酱</v>
       </c>
       <c r="I58" s="14" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="J58" s="9" t="b">
         <v>0</v>
@@ -3984,36 +3990,36 @@
         <v>9</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C2" s="21">
         <v>35000.0</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="I2" s="24" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="J2" s="25" t="b">
         <v>0</v>
@@ -4025,31 +4031,31 @@
     </row>
     <row r="3">
       <c r="A3" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C3" s="21">
         <v>35000.0</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J3" s="25" t="b">
         <v>0</v>
@@ -4061,31 +4067,31 @@
     </row>
     <row r="4">
       <c r="A4" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C4" s="21">
         <v>35000.0</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="J4" s="25" t="b">
         <v>0</v>
@@ -4097,31 +4103,31 @@
     </row>
     <row r="5">
       <c r="A5" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C5" s="21">
         <v>35000.0</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F5" s="23" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G5" s="23" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H5" s="23" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="J5" s="25" t="b">
         <v>0</v>
@@ -4133,31 +4139,31 @@
     </row>
     <row r="6">
       <c r="A6" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C6" s="21">
         <v>35000.0</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="G6" s="23" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H6" s="23" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="J6" s="25" t="b">
         <v>0</v>
@@ -4169,31 +4175,31 @@
     </row>
     <row r="7">
       <c r="A7" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C7" s="21">
         <v>35000.0</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="J7" s="25" t="b">
         <v>0</v>
@@ -4205,31 +4211,31 @@
     </row>
     <row r="8">
       <c r="A8" s="19" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C8" s="21">
         <v>35000.0</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="H8" s="23" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="J8" s="25" t="b">
         <v>0</v>
@@ -4241,31 +4247,31 @@
     </row>
     <row r="9">
       <c r="A9" s="19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C9" s="21">
         <v>35000.0</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="J9" s="25" t="b">
         <v>0</v>
@@ -4277,31 +4283,31 @@
     </row>
     <row r="10">
       <c r="A10" s="19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C10" s="21">
         <v>35000.0</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E10" s="23" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H10" s="23" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="J10" s="25" t="b">
         <v>0</v>
@@ -4313,31 +4319,31 @@
     </row>
     <row r="11">
       <c r="A11" s="19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C11" s="21">
         <v>35000.0</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H11" s="23" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="J11" s="25" t="b">
         <v>0</v>
@@ -4349,31 +4355,31 @@
     </row>
     <row r="12">
       <c r="A12" s="19" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C12" s="21">
         <v>35000.0</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H12" s="23" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="J12" s="25" t="b">
         <v>0</v>
@@ -4385,28 +4391,28 @@
     </row>
     <row r="13">
       <c r="A13" s="27" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C13" s="29">
         <v>35000.0</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="33" t="b">
@@ -4419,25 +4425,25 @@
     </row>
     <row r="14">
       <c r="A14" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C14" s="21">
         <v>30000.0</v>
       </c>
       <c r="D14" s="35"/>
       <c r="E14" s="23" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F14" s="23"/>
       <c r="G14" s="23" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="H14" s="23"/>
       <c r="I14" s="24" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="J14" s="25" t="b">
         <v>0</v>
@@ -4449,25 +4455,25 @@
     </row>
     <row r="15">
       <c r="A15" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C15" s="21">
         <v>30000.0</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="23" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F15" s="23"/>
       <c r="G15" s="23" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H15" s="23"/>
       <c r="I15" s="24" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="J15" s="25" t="b">
         <v>0</v>
@@ -4479,25 +4485,25 @@
     </row>
     <row r="16">
       <c r="A16" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C16" s="21">
         <v>30000.0</v>
       </c>
       <c r="D16" s="35"/>
       <c r="E16" s="23" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="23" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H16" s="23"/>
       <c r="I16" s="24" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="J16" s="25" t="b">
         <v>0</v>
@@ -4509,25 +4515,25 @@
     </row>
     <row r="17">
       <c r="A17" s="19" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C17" s="21">
         <v>30000.0</v>
       </c>
       <c r="D17" s="35"/>
       <c r="E17" s="23" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="F17" s="23"/>
       <c r="G17" s="23" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="H17" s="23"/>
       <c r="I17" s="24" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="J17" s="25" t="b">
         <v>0</v>
@@ -4539,25 +4545,25 @@
     </row>
     <row r="18">
       <c r="A18" s="19" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C18" s="21">
         <v>35000.0</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="23" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="F18" s="23"/>
       <c r="G18" s="23" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="H18" s="23"/>
       <c r="I18" s="24" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="J18" s="25" t="b">
         <v>0</v>
@@ -4569,25 +4575,25 @@
     </row>
     <row r="19">
       <c r="A19" s="19" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C19" s="21">
         <v>35000.0</v>
       </c>
       <c r="D19" s="35"/>
       <c r="E19" s="23" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F19" s="23"/>
       <c r="G19" s="23" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H19" s="23"/>
       <c r="I19" s="24" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="J19" s="25" t="b">
         <v>0</v>
@@ -4599,28 +4605,28 @@
     </row>
     <row r="20">
       <c r="A20" s="19" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C20" s="21">
         <v>20000.0</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H20" s="23" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I20" s="35"/>
       <c r="J20" s="25" t="b">
@@ -4633,28 +4639,28 @@
     </row>
     <row r="21">
       <c r="A21" s="19" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C21" s="21">
         <v>25000.0</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G21" s="23" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="H21" s="23" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I21" s="35"/>
       <c r="J21" s="25" t="b">
@@ -4667,28 +4673,28 @@
     </row>
     <row r="22">
       <c r="A22" s="19" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C22" s="21">
         <v>35000.0</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F22" s="23" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="G22" s="23" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="H22" s="23" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="I22" s="35"/>
       <c r="J22" s="25" t="b">
@@ -4701,28 +4707,28 @@
     </row>
     <row r="23">
       <c r="A23" s="19" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C23" s="21">
         <v>35000.0</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F23" s="23" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="G23" s="23" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="H23" s="23" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="I23" s="35"/>
       <c r="J23" s="25" t="b">
@@ -4735,21 +4741,21 @@
     </row>
     <row r="24">
       <c r="A24" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C24" s="21">
         <v>18000.0</v>
       </c>
       <c r="D24" s="35"/>
       <c r="E24" s="23" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="F24" s="23"/>
       <c r="G24" s="23" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="H24" s="23"/>
       <c r="I24" s="35"/>
@@ -4763,21 +4769,21 @@
     </row>
     <row r="25">
       <c r="A25" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C25" s="21">
         <v>18000.0</v>
       </c>
       <c r="D25" s="35"/>
       <c r="E25" s="23" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25" s="23" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="H25" s="23"/>
       <c r="I25" s="35"/>
@@ -4791,21 +4797,21 @@
     </row>
     <row r="26">
       <c r="A26" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C26" s="37">
         <v>18000.0</v>
       </c>
       <c r="D26" s="35"/>
       <c r="E26" s="23" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="F26" s="23"/>
       <c r="G26" s="23" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="H26" s="23"/>
       <c r="I26" s="35"/>
@@ -4819,21 +4825,21 @@
     </row>
     <row r="27">
       <c r="A27" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C27" s="21">
         <v>18000.0</v>
       </c>
       <c r="D27" s="35"/>
       <c r="E27" s="23" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="F27" s="23"/>
       <c r="G27" s="23" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="H27" s="23"/>
       <c r="I27" s="35"/>
@@ -4847,21 +4853,21 @@
     </row>
     <row r="28">
       <c r="A28" s="19" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C28" s="21">
         <v>12000.0</v>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="23" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="23" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="H28" s="23"/>
       <c r="I28" s="35"/>
@@ -4914,7 +4920,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="39" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B1" s="39" t="s">
         <v>1</v>
@@ -4922,7 +4928,7 @@
     </row>
     <row r="2">
       <c r="A2" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B2" s="39" t="s">
         <v>10</v>
@@ -4930,15 +4936,15 @@
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B4" s="39" t="s">
         <v>53</v>
@@ -4946,47 +4952,47 @@
     </row>
     <row r="5">
       <c r="A5" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B10" s="39" t="s">
         <v>27</v>
@@ -4994,58 +5000,58 @@
     </row>
     <row r="11">
       <c r="A11" s="39" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="39" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -5070,10 +5076,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="39" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="2">

</xml_diff>

<commit_message>
highres banner and dashboard
</commit_message>
<xml_diff>
--- a/public/data/menu.xlsx
+++ b/public/data/menu.xlsx
@@ -2011,8 +2011,8 @@
       </c>
       <c r="F13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D13&lt;&gt;"""", GOOGLETRANSLATE(D13, ""vi"", ""en""), """")
-"),"Filled with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce")</f>
-        <v>Filled with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce</v>
+"),"Stuffed with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce")</f>
+        <v>Stuffed with assorted potatoes, carrots, wood ear mushrooms, corn, green beans, served with sweet and sour fish sauce</v>
       </c>
       <c r="G13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B13,""vi"",""zh"")"),"春卷")</f>
@@ -2020,8 +2020,8 @@
       </c>
       <c r="H13" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D13&lt;&gt;"""", GOOGLETRANSLATE(D13, ""vi"", ""zh""), """")
-"),"馅料为什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露")</f>
-        <v>馅料为什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露</v>
+"),"塞满什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露")</f>
+        <v>塞满什锦土豆、胡萝卜、木耳、玉米、青豆，配糖醋鱼露</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>57</v>
@@ -2220,8 +2220,8 @@
         <v>Lolot leaves rolled with stir-fried mixed mushrooms, rolled with rice paper with fresh vermicelli, assorted raw vegetables, served with vegetarian seasoning sauce</v>
       </c>
       <c r="G18" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""vi"",""zh"")"),"洛洛叶烤蘑菇")</f>
-        <v>洛洛叶烤蘑菇</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B18,""vi"",""zh"")"),"槟榔叶烤蘑菇")</f>
+        <v>槟榔叶烤蘑菇</v>
       </c>
       <c r="H18" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D18&lt;&gt;"""", GOOGLETRANSLATE(D18, ""vi"", ""zh""), """")
@@ -2257,8 +2257,8 @@
       </c>
       <c r="F19" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D19&lt;&gt;"""", GOOGLETRANSLATE(D19, ""vi"", ""en""), """")
-"),"green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushrooms ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli")</f>
-        <v>green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushrooms ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli</v>
+"),"green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushroom ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli")</f>
+        <v>green pepper hotpot ; spinach ; Chinese cabbage ; mustard greens ; chicken drumstick mushrooms ; abalone mushrooms ; Enoki mushroom ; soft tofu ; Served with vegetarian fish sauce and fresh vermicelli</v>
       </c>
       <c r="G19" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B19,""vi"",""zh"")"),"青椒蘑菇火锅")</f>
@@ -2298,8 +2298,8 @@
       </c>
       <c r="F20" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D20&lt;&gt;"""", GOOGLETRANSLATE(D20, ""vi"", ""en""), """")
-"),"Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushrooms ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli")</f>
-        <v>Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushrooms ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli</v>
+"),"Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushroom ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli")</f>
+        <v>Thai hotpot ; banana vegetables ; Chinese cabbage ; spinach ; Vegetables need water; chicken drumstick mushrooms ; Enoki mushroom ; abalone mushrooms ; Soft tofu served with vegetarian fish sauce and fresh vermicelli</v>
       </c>
       <c r="G20" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B20,""vi"",""zh"")"),"泰式火锅")</f>
@@ -3196,8 +3196,8 @@
         <v>fairy hair ; American corn ; carrot ; mushroom ; string beans ; onions ; pepper ; coriander</v>
       </c>
       <c r="G42" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""vi"",""zh"")"),"东天汤")</f>
-        <v>东天汤</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B42,""vi"",""zh"")"),"TOC天汤")</f>
+        <v>TOC天汤</v>
       </c>
       <c r="H42" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D42&lt;&gt;"""", GOOGLETRANSLATE(D42, ""vi"", ""zh""), """")
@@ -3442,8 +3442,8 @@
         <v>kimchi hotpot ; purple cabbage ; Chinese cabbage ; Abalone mushrooms served with Korean noodles</v>
       </c>
       <c r="G48" s="4" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""vi"",""zh"")"),"肚肚配辣椒蘑菇酱")</f>
-        <v>肚肚配辣椒蘑菇酱</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B48,""vi"",""zh"")"),"肚腩配辣椒蘑菇酱")</f>
+        <v>肚腩配辣椒蘑菇酱</v>
       </c>
       <c r="H48" s="4" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("IF(D48&lt;&gt;"""", GOOGLETRANSLATE(D48, ""vi"", ""zh""), """")

</xml_diff>